<commit_message>
Change R24 to 10k, R26 to 30k to correct input/output meter reference levels
</commit_message>
<xml_diff>
--- a/dmeter/BoM.xlsx
+++ b/dmeter/BoM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tom\Documents\Electronics\amtx\Audio\amproc\dmeter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6399A6FF-03D0-4302-B1BB-CEE4169EB498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2C6B59-0978-452B-B3EF-EAF35A4F2BA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="7275" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -91,9 +91,6 @@
     <t xml:space="preserve">R20 R18 </t>
   </si>
   <si>
-    <t xml:space="preserve">R24 </t>
-  </si>
-  <si>
     <t>30k</t>
   </si>
   <si>
@@ -469,9 +466,6 @@
     <t>RV1 RV2 RV3</t>
   </si>
   <si>
-    <t>R13 R10 R15 R8 R17 R14 R12 R16 R9 R19 R25 R26 R27</t>
-  </si>
-  <si>
     <t>T93YA</t>
   </si>
   <si>
@@ -482,6 +476,12 @@
   </si>
   <si>
     <t>1141404</t>
+  </si>
+  <si>
+    <t>R26</t>
+  </si>
+  <si>
+    <t>R13 R10 R15 R8 R17 R14 R12 R16 R9 R19 R24 R25 R27</t>
   </si>
 </sst>
 </file>
@@ -1341,7 +1341,7 @@
   <dimension ref="A1:L47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD26"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1361,37 +1361,37 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.4">
@@ -1405,19 +1405,19 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" t="s">
         <v>53</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>54</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>55</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>56</v>
-      </c>
-      <c r="H2" t="s">
-        <v>57</v>
       </c>
       <c r="I2">
         <v>2068981</v>
@@ -1441,22 +1441,22 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" t="s">
         <v>58</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" t="s">
         <v>59</v>
       </c>
-      <c r="F3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>60</v>
       </c>
-      <c r="H3" t="s">
-        <v>61</v>
-      </c>
       <c r="I3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J3">
         <v>0.46500000000000002</v>
@@ -1477,22 +1477,22 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" t="s">
         <v>62</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>63</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>64</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I4" t="s">
         <v>65</v>
-      </c>
-      <c r="H4" t="s">
-        <v>57</v>
-      </c>
-      <c r="I4" t="s">
-        <v>66</v>
       </c>
       <c r="J4">
         <v>8.2299999999999998E-2</v>
@@ -1513,22 +1513,22 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" t="s">
         <v>67</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" t="s">
         <v>68</v>
       </c>
-      <c r="F5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I5" t="s">
         <v>69</v>
-      </c>
-      <c r="H5" t="s">
-        <v>57</v>
-      </c>
-      <c r="I5" t="s">
-        <v>70</v>
       </c>
       <c r="J5">
         <v>9.7000000000000003E-2</v>
@@ -1549,22 +1549,22 @@
         <v>10</v>
       </c>
       <c r="D6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" t="s">
         <v>71</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>72</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>73</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I6" t="s">
         <v>74</v>
-      </c>
-      <c r="H6" t="s">
-        <v>57</v>
-      </c>
-      <c r="I6" t="s">
-        <v>75</v>
       </c>
       <c r="J6">
         <v>3.1899999999999998E-2</v>
@@ -1576,7 +1576,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -1585,22 +1585,22 @@
         <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E7" t="s">
+        <v>139</v>
+      </c>
+      <c r="F7" t="s">
+        <v>72</v>
+      </c>
+      <c r="G7" t="s">
         <v>140</v>
       </c>
-      <c r="F7" t="s">
-        <v>73</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
+        <v>56</v>
+      </c>
+      <c r="I7" t="s">
         <v>141</v>
-      </c>
-      <c r="H7" t="s">
-        <v>57</v>
-      </c>
-      <c r="I7" t="s">
-        <v>142</v>
       </c>
       <c r="J7">
         <v>9.5799999999999996E-2</v>
@@ -1612,7 +1612,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -1621,22 +1621,22 @@
         <v>12</v>
       </c>
       <c r="D8" t="s">
+        <v>132</v>
+      </c>
+      <c r="E8" t="s">
         <v>133</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
+        <v>72</v>
+      </c>
+      <c r="G8" t="s">
         <v>134</v>
       </c>
-      <c r="F8" t="s">
-        <v>73</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I8" t="s">
         <v>135</v>
-      </c>
-      <c r="H8" t="s">
-        <v>57</v>
-      </c>
-      <c r="I8" t="s">
-        <v>136</v>
       </c>
       <c r="J8">
         <v>6.0900000000000003E-2</v>
@@ -1648,7 +1648,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B9">
         <v>20</v>
@@ -1657,22 +1657,22 @@
         <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E9" t="s">
+        <v>142</v>
+      </c>
+      <c r="F9" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" t="s">
         <v>143</v>
       </c>
-      <c r="F9" t="s">
-        <v>73</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
+        <v>56</v>
+      </c>
+      <c r="I9" t="s">
         <v>144</v>
-      </c>
-      <c r="H9" t="s">
-        <v>57</v>
-      </c>
-      <c r="I9" t="s">
-        <v>145</v>
       </c>
       <c r="J9">
         <v>7.46E-2</v>
@@ -1693,22 +1693,22 @@
         <v>15</v>
       </c>
       <c r="D10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" t="s">
         <v>76</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>77</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>78</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I10" t="s">
         <v>79</v>
-      </c>
-      <c r="H10" t="s">
-        <v>57</v>
-      </c>
-      <c r="I10" t="s">
-        <v>80</v>
       </c>
       <c r="J10">
         <v>0.247</v>
@@ -1718,7 +1718,7 @@
         <v>0.247</v>
       </c>
       <c r="L10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.4">
@@ -1732,22 +1732,22 @@
         <v>17</v>
       </c>
       <c r="D11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E11" t="s">
         <v>82</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>83</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>84</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I11" t="s">
         <v>85</v>
-      </c>
-      <c r="H11" t="s">
-        <v>57</v>
-      </c>
-      <c r="I11" t="s">
-        <v>86</v>
       </c>
       <c r="J11">
         <v>0.16400000000000001</v>
@@ -1768,22 +1768,22 @@
         <v>19</v>
       </c>
       <c r="D12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E12" t="s">
         <v>87</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
+        <v>72</v>
+      </c>
+      <c r="G12" t="s">
         <v>88</v>
       </c>
-      <c r="F12" t="s">
-        <v>73</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
+        <v>56</v>
+      </c>
+      <c r="I12" t="s">
         <v>89</v>
-      </c>
-      <c r="H12" t="s">
-        <v>57</v>
-      </c>
-      <c r="I12" t="s">
-        <v>90</v>
       </c>
       <c r="J12">
         <v>3.0300000000000001E-2</v>
@@ -1804,22 +1804,22 @@
         <v>390</v>
       </c>
       <c r="D13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E13" t="s">
+        <v>90</v>
+      </c>
+      <c r="F13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G13" t="s">
         <v>91</v>
       </c>
-      <c r="F13" t="s">
-        <v>73</v>
-      </c>
-      <c r="G13" t="s">
-        <v>92</v>
-      </c>
       <c r="H13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J13">
         <v>2.8799999999999999E-2</v>
@@ -1831,7 +1831,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -1840,22 +1840,22 @@
         <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F14" t="s">
+        <v>72</v>
+      </c>
+      <c r="G14" t="s">
         <v>95</v>
       </c>
-      <c r="F14" t="s">
-        <v>73</v>
-      </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
+        <v>56</v>
+      </c>
+      <c r="I14" t="s">
         <v>96</v>
-      </c>
-      <c r="H14" t="s">
-        <v>57</v>
-      </c>
-      <c r="I14" t="s">
-        <v>97</v>
       </c>
       <c r="J14">
         <v>2.8799999999999999E-2</v>
@@ -1873,25 +1873,25 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
+        <v>97</v>
+      </c>
+      <c r="D15" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15" t="s">
         <v>98</v>
       </c>
-      <c r="D15" t="s">
-        <v>87</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
+        <v>72</v>
+      </c>
+      <c r="G15" t="s">
         <v>99</v>
       </c>
-      <c r="F15" t="s">
-        <v>73</v>
-      </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I15" t="s">
         <v>100</v>
-      </c>
-      <c r="H15" t="s">
-        <v>57</v>
-      </c>
-      <c r="I15" t="s">
-        <v>101</v>
       </c>
       <c r="J15">
         <v>0.03</v>
@@ -1903,31 +1903,31 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>152</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J16">
         <v>3.0700000000000002E-2</v>
@@ -1939,31 +1939,31 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17">
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G17" t="s">
+        <v>110</v>
+      </c>
+      <c r="H17" t="s">
+        <v>56</v>
+      </c>
+      <c r="I17" t="s">
         <v>111</v>
-      </c>
-      <c r="H17" t="s">
-        <v>57</v>
-      </c>
-      <c r="I17" t="s">
-        <v>112</v>
       </c>
       <c r="J17">
         <v>2.81E-2</v>
@@ -1975,7 +1975,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18">
         <v>4</v>
@@ -1984,22 +1984,22 @@
         <v>100</v>
       </c>
       <c r="D18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E18" t="s">
+        <v>112</v>
+      </c>
+      <c r="F18" t="s">
+        <v>72</v>
+      </c>
+      <c r="G18" t="s">
+        <v>92</v>
+      </c>
+      <c r="H18" t="s">
+        <v>56</v>
+      </c>
+      <c r="I18" t="s">
         <v>113</v>
-      </c>
-      <c r="F18" t="s">
-        <v>73</v>
-      </c>
-      <c r="G18" t="s">
-        <v>93</v>
-      </c>
-      <c r="H18" t="s">
-        <v>57</v>
-      </c>
-      <c r="I18" t="s">
-        <v>114</v>
       </c>
       <c r="J18">
         <v>0.03</v>
@@ -2011,31 +2011,31 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G19" t="s">
+        <v>114</v>
+      </c>
+      <c r="H19" t="s">
+        <v>56</v>
+      </c>
+      <c r="I19" t="s">
         <v>115</v>
-      </c>
-      <c r="H19" t="s">
-        <v>57</v>
-      </c>
-      <c r="I19" t="s">
-        <v>116</v>
       </c>
       <c r="J19">
         <v>0.03</v>
@@ -2047,31 +2047,31 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G20" t="s">
+        <v>116</v>
+      </c>
+      <c r="H20" t="s">
+        <v>56</v>
+      </c>
+      <c r="I20" t="s">
         <v>117</v>
-      </c>
-      <c r="H20" t="s">
-        <v>57</v>
-      </c>
-      <c r="I20" t="s">
-        <v>118</v>
       </c>
       <c r="J20">
         <v>3.0200000000000001E-2</v>
@@ -2083,31 +2083,31 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G21" t="s">
+        <v>118</v>
+      </c>
+      <c r="H21" t="s">
+        <v>56</v>
+      </c>
+      <c r="I21" t="s">
         <v>119</v>
-      </c>
-      <c r="H21" t="s">
-        <v>57</v>
-      </c>
-      <c r="I21" t="s">
-        <v>120</v>
       </c>
       <c r="J21">
         <v>2.8400000000000002E-2</v>
@@ -2119,31 +2119,31 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J22">
         <v>2.86E-2</v>
@@ -2155,31 +2155,31 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G23" t="s">
+        <v>121</v>
+      </c>
+      <c r="H23" t="s">
+        <v>56</v>
+      </c>
+      <c r="I23" t="s">
         <v>122</v>
-      </c>
-      <c r="H23" t="s">
-        <v>57</v>
-      </c>
-      <c r="I23" t="s">
-        <v>123</v>
       </c>
       <c r="J23">
         <v>2.6599999999999999E-2</v>
@@ -2191,7 +2191,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B24">
         <v>3</v>
@@ -2200,22 +2200,22 @@
         <v>21</v>
       </c>
       <c r="D24" t="s">
+        <v>148</v>
+      </c>
+      <c r="E24" t="s">
+        <v>149</v>
+      </c>
+      <c r="F24" t="s">
+        <v>63</v>
+      </c>
+      <c r="G24" t="s">
         <v>150</v>
       </c>
-      <c r="E24" t="s">
+      <c r="H24" t="s">
+        <v>56</v>
+      </c>
+      <c r="I24" t="s">
         <v>151</v>
-      </c>
-      <c r="F24" t="s">
-        <v>64</v>
-      </c>
-      <c r="G24" t="s">
-        <v>152</v>
-      </c>
-      <c r="H24" t="s">
-        <v>57</v>
-      </c>
-      <c r="I24" t="s">
-        <v>153</v>
       </c>
       <c r="J24">
         <v>1.44</v>
@@ -2227,31 +2227,31 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25">
         <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D25" t="s">
+        <v>123</v>
+      </c>
+      <c r="E25" t="s">
         <v>124</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>125</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>126</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
+        <v>56</v>
+      </c>
+      <c r="I25" t="s">
         <v>127</v>
-      </c>
-      <c r="H25" t="s">
-        <v>57</v>
-      </c>
-      <c r="I25" t="s">
-        <v>128</v>
       </c>
       <c r="J25">
         <v>0.90500000000000003</v>
@@ -2263,31 +2263,31 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26">
         <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D26" t="s">
+        <v>128</v>
+      </c>
+      <c r="E26" t="s">
         <v>129</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
+        <v>125</v>
+      </c>
+      <c r="G26" t="s">
         <v>130</v>
       </c>
-      <c r="F26" t="s">
-        <v>126</v>
-      </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
+        <v>56</v>
+      </c>
+      <c r="I26" t="s">
         <v>131</v>
-      </c>
-      <c r="H26" t="s">
-        <v>57</v>
-      </c>
-      <c r="I26" t="s">
-        <v>132</v>
       </c>
       <c r="J26">
         <v>0.47699999999999998</v>
@@ -2303,7 +2303,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.4">
       <c r="J28" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K28" s="6">
         <f>SUM(K2:K26)</f>

</xml_diff>